<commit_message>
[#38] CreateNutrition api 구현
</commit_message>
<xml_diff>
--- a/backend/dataFiles/G_Order 데이터정리.xlsx
+++ b/backend/dataFiles/G_Order 데이터정리.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.10097"/>
+  <x:fileVersion appName="HCell" lastEdited="11.0" lowestEdited="11.0" rupBuild="0.4167"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="11835" tabRatio="580"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="8232" tabRatio="580" activeTab="3"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="전체" sheetId="1" r:id="rId4"/>
@@ -26,477 +26,480 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="157">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="158">
+  <x:si>
+    <x:t>탄수화물: 20g, 단백질: 4g, 지방: 7g, 나트륨: 50mg, 콜레스테롤: 35mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로메인 상추: 100g, 크루통: 20g, 파마산 치즈: 30g, 시저 드레핑: 30ml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 20g, 단백질: 3g, 지방: 15g, 나트륨: 40mg, 콜레스테롤: 50mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>바게트: 50g, 토마토: 75g, 바질: 2잎, 올리브 오일: 15ml, 마늘: 2g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 50g, 단백질: 8g, 지방: 10g, 나트륨: 400mg, 콜레스테롤: 0mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 20g, 단백질: 3g, 지방: 5g, 나트륨: 200mg, 콜레스테롤: 0g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 25g, 단백질: 4g, 지방: 3g, 나트륨: 300mg, 콜레스테롤: 0mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루: 100g, 바질: 30g, 올리브 오일: 30ml, 치즈: 30g, 잣: 10g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://cdn.imweb.me/thumbnail/20220623/417baec03c622.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://static.wtable.co.kr/image-resize/production/service/recipe/1886/16x9/fff78c8b-be96-44f0-bd91-653a5d297b8c.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.unileverfoodsolutions.co.kr/dam/global-ufs/mcos/south-korea/calcmenu/recipes/kr-recipes/western/header/%EB%AF%B8%EB%84%A4%EC%8A%A4%ED%8A%B8%EB%A1%9C%EB%84%A4-minestrone-soup-header.png</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.dongsuh.co.kr/2017/images/page/03_mediaCenter/img_class_3_2_1_1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://static.wtable.co.kr/image-resize/production/service/recipe/100/4x3/6821ee02-5846-4f9e-a4b8-7cf9b549126b.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://i.namu.wiki/i/tf5DuJNrtIkYP0srIDkAPyk6rAI6lvHEIPAxrygx1v8FDap_e_K0W4Ecg1id4Dm22YQzLP9LaS0mXwmfBSdMdQ.webp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://i.namu.wiki/i/g3Rt4-oE30JuiJRDQOJcPi9PGdfAmqEUAk_2zdloaaqqBKWpYGHMZdE6jbqB0-KUEL-tKt9blS2o9QEqlITE5g.webp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 6g, 단백질: 10g, 지방: 14g, 나트륨: 300mg, 콜레스테롤: 30mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 10g, 닥배질: 7g, 지방: 15g, 나트륨: 350mg, 콜레스테롤: 20mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 35g, 단백질: 10g, 지방: 20g, 나트륨: 400mg, 콜레스테롤: 60mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 45g, 단백질: 12g, 지방: 15g, 나트륨: 600mg, 콜레스테롤: 25mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 40g, 단백질: 15g, 지방: 18g, 나트륨: 500mg, 콜레스테롤: 50mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루: 100g, 소고기: 100g, 토마토 소스: 100ml, 양파: 50g, 마늘: 2g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 35g, 단백질: 8g, 지방: 25g, 나트륨: 350mg, 콜레스테롤: 15mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 45g, 단백질: 15g, 지방: 12g, 나트륨: 450mg, 콜레스테롤: 70mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로메인 상추, 크루통, 파마산 치즈, 시저 드레싱</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루, 소고기, 토마토 소스, 양파, 마늘</x:t>
+  </x:si>
+  <x:si>
+    <x:t>바게트, 토마토, 바질, 올리브 오일, 마늘</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://img.freepik.com/premium-photo/photo-chicken-alfredo-pasta_933496-17781.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>토마토: 150g, 치즈: 100g, 바질: 4잎, 올리브 오일: 15ml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루: 150g, 토마토 소스: 50ml, 치즈: 100g, 바질: 4잎</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루: 150g, 올리브 오일: 30ml, 로즈마리: 2g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쌀: 100g, 새우: 100g, 크림: 50ml, 치즈: 30g, 양파: 50g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>토마토: 75g, 당근: 50g, 셀러리: 50g, 양파: 50g, 밀가루: 30g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/43/Focaccia-erbe-olive.jpg/640px-Focaccia-erbe-olive.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>우유: 100ml, 설탕: 50g, 계란: 1개, 바닐라: 5ml</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루: 100g, 크림: 100ml, 치즈: 50g, 버터: 15G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>크림: 100ml, 설탕: 30g, 바닐라: 5ml, 젤라틴: 2g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bruschetta-&gt;브루스케타, caprese_salad-&gt;카프레제 샐러드, caesar_salad-&gt;시저 샐러드, maragherita_pizza-&gt;마르게리타 피자, alfredo_pasta-&gt;알프레도 파스타, bolognese_spaghetti-&gt;볼로네제 스파게티, shrimp_risotto-&gt;새우 리조또, focaccia-&gt;포카치아, minestrone_soup-&gt;미네스트로네 수프, gelato-&gt;젤라토, panna_cotta-&gt;판나 코타, pesto_pasta-&gt;페스토 파스타, espresso-&gt;에스프레소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2018/07/22/3bc1856e3d0263519df771f6dea327dc1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2020/07/15/45a490d842275b5473636b561201b0131.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2020/06/25/0aff91e3dbc15d35d3df52c952177f541.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2019/01/04/7806a1394260cfcd7a4878de87071e321.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>caesar_salad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루, 크림, 치즈, 버터</x:t>
+  </x:si>
+  <x:si>
+    <x:t>romain_lettuce</x:t>
+  </x:si>
+  <x:si>
+    <x:t>carbohydrate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ingredient_id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tomato_sauce</x:t>
+  </x:si>
+  <x:si>
+    <x:t>caesar_dressing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shrimp_risotto</x:t>
+  </x:si>
+  <x:si>
+    <x:t>alfredo_pasta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>caprese_salad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>우유, 설탕, 계란, 바닐라</x:t>
+  </x:si>
+  <x:si>
+    <x:t>minestrone_soup</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nutrition_id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>romaine_lettuce</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀, 유제품, 견과류, 생선</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루, 올리브 오일, 로즈마리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>allergy_occurrence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bolognese_spaghetti</x:t>
+  </x:si>
+  <x:si>
+    <x:t>쌀, 새우, 크림, 치즈, 양파</x:t>
+  </x:si>
+  <x:si>
+    <x:t>토마토, 치즈, 바질, 올리브 오일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>크림, 설탕, 바닐라, 젤라틴</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루, 토마토 소스, 치즈, 바질</x:t>
+  </x:si>
+  <x:si>
+    <x:t>maragherita_pizza</x:t>
+  </x:si>
+  <x:si>
+    <x:t>토마토, 당근, 셀러리, 양파, 밀가루</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀가루, 바질, 올리브 오일, 치즈, 잣</x:t>
+  </x:si>
+  <x:si>
+    <x:t>coffee_bean</x:t>
+  </x:si>
+  <x:si>
+    <x:t>마르게리타 피자</x:t>
+  </x:si>
+  <x:si>
+    <x:t>category</x:t>
+  </x:si>
+  <x:si>
+    <x:t>olive_oil</x:t>
+  </x:si>
+  <x:si>
+    <x:t>baguette</x:t>
+  </x:si>
+  <x:si>
+    <x:t>allergy_id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cholesterol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>expresso</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rosemary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>image_url</x:t>
+  </x:si>
+  <x:si>
+    <x:t>appetizer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀, 유제품, 대두</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pesto_pasta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>order_count</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">알프레도 파스타 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_dish</x:t>
+  </x:si>
+  <x:si>
+    <x:t>미네스트로네 수프</x:t>
+  </x:si>
+  <x:si>
+    <x:t>panna_cotta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유제품, 계란, 대두</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sold_out</x:t>
+  </x:si>
+  <x:si>
+    <x:t>볼로네제 스파게티</x:t>
+  </x:si>
+  <x:si>
+    <x:t>total_price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀, 유제품, 겨자</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shellfish</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pine_nut</x:t>
+  </x:si>
+  <x:si>
+    <x:t>focaccia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bruschetta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>갑각류, 유제품</x:t>
+  </x:si>
+  <x:si>
+    <x:t>카프레제 샐러드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>탄수화물: 2g, 단백질: 0g, 지방: 0g, 나트륨: 5mg, 콜레스테롤: 0mg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>butter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cheese</x:t>
+  </x:si>
+  <x:si>
+    <x:t>원두: 8g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rice</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gelatin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>crouton</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tomato</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gelato</x:t>
+  </x:si>
+  <x:si>
+    <x:t>price</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dairy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cream</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fish</x:t>
+  </x:si>
+  <x:si>
+    <x:t>시저 샐러드</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀, 유제품</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mustard</x:t>
+  </x:si>
+  <x:si>
+    <x:t>판나 코타</x:t>
+  </x:si>
+  <x:si>
+    <x:t>페스토 파스타</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에스프레소</x:t>
+  </x:si>
+  <x:si>
+    <x:t>영양 성분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>abc123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dessert</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알레르기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>menu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>beef</x:t>
+  </x:si>
+  <x:si>
+    <x:t>carrot</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">새우 리조또 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>coupon</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">브루스케타 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>basil</x:t>
+  </x:si>
+  <x:si>
+    <x:t>milk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sodium</x:t>
+  </x:si>
+  <x:si>
+    <x:t>onion</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shrimp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sugar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>celery</x:t>
+  </x:si>
+  <x:si>
+    <x:t>셀러리, 밀</x:t>
+  </x:si>
+  <x:si>
+    <x:t>protein</x:t>
+  </x:si>
+  <x:si>
+    <x:t>flour</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vanilla</x:t>
+  </x:si>
+  <x:si>
+    <x:t>재료 양</x:t>
+  </x:si>
+  <x:si>
+    <x:t>메인디쉬</x:t>
+  </x:si>
+  <x:si>
+    <x:t>포카치아</x:t>
+  </x:si>
+  <x:si>
+    <x:t>userID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>에피타이저</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gluten</x:t>
+  </x:si>
+  <x:si>
+    <x:t>garlic</x:t>
+  </x:si>
+  <x:si>
+    <x:t>밀</x:t>
+  </x:si>
   <x:si>
     <x:t>원두</x:t>
   </x:si>
   <x:si>
-    <x:t>밀</x:t>
+    <x:t>메뉴</x:t>
   </x:si>
   <x:si>
     <x:t>없음</x:t>
   </x:si>
   <x:si>
+    <x:t>nut</x:t>
+  </x:si>
+  <x:si>
+    <x:t>구분</x:t>
+  </x:si>
+  <x:si>
+    <x:t>재료</x:t>
+  </x:si>
+  <x:si>
     <x:t>fat</x:t>
   </x:si>
   <x:si>
-    <x:t>nut</x:t>
+    <x:t>디저트</x:t>
+  </x:si>
+  <x:si>
+    <x:t>id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이미지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유제품</x:t>
   </x:si>
   <x:si>
     <x:t>젤라토</x:t>
   </x:si>
   <x:si>
-    <x:t>id</x:t>
-  </x:si>
-  <x:si>
     <x:t>egg</x:t>
   </x:si>
   <x:si>
-    <x:t>디저트</x:t>
-  </x:si>
-  <x:si>
     <x:t>soy</x:t>
   </x:si>
   <x:si>
-    <x:t>구분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유제품</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 20g, 단백질: 3g, 지방: 15g, 나트륨: 40mg, 콜레스테롤: 50mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로메인 상추: 100g, 크루통: 20g, 파마산 치즈: 30g, 시저 드레핑: 30ml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 20g, 단백질: 4g, 지방: 7g, 나트륨: 50mg, 콜레스테롤: 35mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>바게트: 50g, 토마토: 75g, 바질: 2잎, 올리브 오일: 15ml, 마늘: 2g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 25g, 단백질: 4g, 지방: 3g, 나트륨: 300mg, 콜레스테롤: 0mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루: 100g, 바질: 30g, 올리브 오일: 30ml, 치즈: 30g, 잣: 10g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 50g, 단백질: 8g, 지방: 10g, 나트륨: 400mg, 콜레스테롤: 0mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 20g, 단백질: 3g, 지방: 5g, 나트륨: 200mg, 콜레스테롤: 0g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://static.wtable.co.kr/image-resize/production/service/recipe/1886/16x9/fff78c8b-be96-44f0-bd91-653a5d297b8c.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>bruschetta-&gt;브루스케타, caprese_salad-&gt;카프레제 샐러드, caesar_salad-&gt;시저 샐러드, maragherita_pizza-&gt;마르게리타 피자, alfredo_pasta-&gt;알프레도 파스타, bolognese_spaghetti-&gt;볼로네제 스파게티, shrimp_risotto-&gt;새우 리조또, focaccia-&gt;포카치아, minestrone_soup-&gt;미네스트로네 수프, gelato-&gt;젤라토, panna_cotta-&gt;판나 코타, pesto_pasta-&gt;페스토 파스타, espresso-&gt;에스프레소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메뉴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이미지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>재료</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://cdn.imweb.me/thumbnail/20220623/417baec03c622.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루: 100g, 크림: 100ml, 치즈: 50g, 버터: 15G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>우유: 100ml, 설탕: 50g, 계란: 1개, 바닐라: 5ml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>크림: 100ml, 설탕: 30g, 바닐라: 5ml, 젤라틴: 2g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루, 바질, 올리브 오일, 치즈, 잣</x:t>
-  </x:si>
-  <x:si>
-    <x:t>토마토, 당근, 셀러리, 양파, 밀가루</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쌀, 새우, 크림, 치즈, 양파</x:t>
-  </x:si>
-  <x:si>
-    <x:t>토마토, 치즈, 바질, 올리브 오일</x:t>
-  </x:si>
-  <x:si>
-    <x:t>allergy_occurrence</x:t>
-  </x:si>
-  <x:si>
-    <x:t>크림, 설탕, 바닐라, 젤라틴</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루, 토마토 소스, 치즈, 바질</x:t>
-  </x:si>
-  <x:si>
-    <x:t>maragherita_pizza</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루, 올리브 오일, 로즈마리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>bolognese_spaghetti</x:t>
-  </x:si>
-  <x:si>
-    <x:t>coffee_bean</x:t>
-  </x:si>
-  <x:si>
-    <x:t>마르게리타 피자</x:t>
-  </x:si>
-  <x:si>
-    <x:t>category</x:t>
-  </x:si>
-  <x:si>
-    <x:t>rosemary</x:t>
-  </x:si>
-  <x:si>
-    <x:t>image_url</x:t>
-  </x:si>
-  <x:si>
-    <x:t>order_count</x:t>
-  </x:si>
-  <x:si>
-    <x:t>pesto_pasta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_dish</x:t>
-  </x:si>
-  <x:si>
-    <x:t>panna_cotta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>미네스트로네 수프</x:t>
-  </x:si>
-  <x:si>
-    <x:t>유제품, 계란, 대두</x:t>
-  </x:si>
-  <x:si>
-    <x:t>olive_oil</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">알프레도 파스타 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀, 유제품, 대두</x:t>
-  </x:si>
-  <x:si>
-    <x:t>baguette</x:t>
-  </x:si>
-  <x:si>
-    <x:t>allergy_id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>cholesterol</x:t>
-  </x:si>
-  <x:si>
-    <x:t>expresso</x:t>
-  </x:si>
-  <x:si>
-    <x:t>appetizer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>total_price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sold_out</x:t>
-  </x:si>
-  <x:si>
-    <x:t>pine_nut</x:t>
-  </x:si>
-  <x:si>
-    <x:t>bruschetta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀, 유제품, 겨자</x:t>
-  </x:si>
-  <x:si>
-    <x:t>갑각류, 유제품</x:t>
-  </x:si>
-  <x:si>
-    <x:t>shellfish</x:t>
-  </x:si>
-  <x:si>
-    <x:t>focaccia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>카프레제 샐러드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>볼로네제 스파게티</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://static.wtable.co.kr/image-resize/production/service/recipe/100/4x3/6821ee02-5846-4f9e-a4b8-7cf9b549126b.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://i.namu.wiki/i/tf5DuJNrtIkYP0srIDkAPyk6rAI6lvHEIPAxrygx1v8FDap_e_K0W4Ecg1id4Dm22YQzLP9LaS0mXwmfBSdMdQ.webp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://i.namu.wiki/i/g3Rt4-oE30JuiJRDQOJcPi9PGdfAmqEUAk_2zdloaaqqBKWpYGHMZdE6jbqB0-KUEL-tKt9blS2o9QEqlITE5g.webp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>쌀: 100g, 새우: 100g, 크림: 50ml, 치즈: 30g, 양파: 50g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>토마토: 75g, 당근: 50g, 셀러리: 50g, 양파: 50g, 밀가루: 30g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 2g, 단백질: 0g, 지방: 0g, 나트륨: 5mg, 콜레스테롤: 0mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 35g, 단백질: 10g, 지방: 20g, 나트륨: 400mg, 콜레스테롤: 60mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 45g, 단백질: 12g, 지방: 15g, 나트륨: 600mg, 콜레스테롤: 25mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 45g, 단백질: 15g, 지방: 12g, 나트륨: 450mg, 콜레스테롤: 70mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 6g, 단백질: 10g, 지방: 14g, 나트륨: 300mg, 콜레스테롤: 30mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 40g, 단백질: 15g, 지방: 18g, 나트륨: 500mg, 콜레스테롤: 50mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루: 100g, 소고기: 100g, 토마토 소스: 100ml, 양파: 50g, 마늘: 2g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 35g, 단백질: 8g, 지방: 25g, 나트륨: 350mg, 콜레스테롤: 15mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>탄수화물: 10g, 닥배질: 7g, 지방: 15g, 나트륨: 350mg, 콜레스테롤: 20mg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/43/Focaccia-erbe-olive.jpg/640px-Focaccia-erbe-olive.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루: 150g, 토마토 소스: 50ml, 치즈: 100g, 바질: 4잎</x:t>
-  </x:si>
-  <x:si>
-    <x:t>토마토: 150g, 치즈: 100g, 바질: 4잎, 올리브 오일: 15ml</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.unileverfoodsolutions.co.kr/dam/global-ufs/mcos/south-korea/calcmenu/recipes/kr-recipes/western/header/%EB%AF%B8%EB%84%A4%EC%8A%A4%ED%8A%B8%EB%A1%9C%EB%84%A4-minestrone-soup-header.png</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.dongsuh.co.kr/2017/images/page/03_mediaCenter/img_class_3_2_1_1.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2020/06/25/0aff91e3dbc15d35d3df52c952177f541.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2018/07/22/3bc1856e3d0263519df771f6dea327dc1.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2020/07/15/45a490d842275b5473636b561201b0131.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://recipe1.ezmember.co.kr/cache/recipe/2019/01/04/7806a1394260cfcd7a4878de87071e321.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>menu</x:t>
-  </x:si>
-  <x:si>
-    <x:t>carrot</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dairy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>시저 샐러드</x:t>
-  </x:si>
-  <x:si>
-    <x:t>페스토 파스타</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알레르기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>beef</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에스프레소</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀, 유제품</x:t>
-  </x:si>
-  <x:si>
-    <x:t>영양 성분</x:t>
-  </x:si>
-  <x:si>
-    <x:t>판나 코타</x:t>
-  </x:si>
-  <x:si>
-    <x:t>abc123</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gelato</x:t>
-  </x:si>
-  <x:si>
-    <x:t>cream</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tomato</x:t>
-  </x:si>
-  <x:si>
-    <x:t>price</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dessert</x:t>
-  </x:si>
-  <x:si>
-    <x:t>fish</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mustard</x:t>
-  </x:si>
-  <x:si>
-    <x:t>protein</x:t>
-  </x:si>
-  <x:si>
-    <x:t>셀러리, 밀</x:t>
-  </x:si>
-  <x:si>
-    <x:t>basil</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">브루스케타 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>sodium</x:t>
-  </x:si>
-  <x:si>
-    <x:t>onion</x:t>
-  </x:si>
-  <x:si>
-    <x:t>flour</x:t>
-  </x:si>
-  <x:si>
-    <x:t>milk</x:t>
-  </x:si>
-  <x:si>
-    <x:t>shrimp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sugar</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">새우 리조또 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>celery</x:t>
-  </x:si>
-  <x:si>
-    <x:t>coupon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루: 150g, 올리브 오일: 30ml, 로즈마리: 2g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루, 소고기, 토마토 소스, 양파, 마늘</x:t>
-  </x:si>
-  <x:si>
-    <x:t>로메인 상추, 크루통, 파마산 치즈, 시저 드레싱</x:t>
-  </x:si>
-  <x:si>
-    <x:t>바게트, 토마토, 바질, 올리브 오일, 마늘</x:t>
-  </x:si>
-  <x:si>
-    <x:t>shrimp_risotto</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀가루, 크림, 치즈, 버터</x:t>
-  </x:si>
-  <x:si>
-    <x:t>alfredo_pasta</x:t>
-  </x:si>
-  <x:si>
-    <x:t>carbohydrate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>tomato_sauce</x:t>
-  </x:si>
-  <x:si>
-    <x:t>caesar_salad</x:t>
-  </x:si>
-  <x:si>
-    <x:t>우유, 설탕, 계란, 바닐라</x:t>
-  </x:si>
-  <x:si>
-    <x:t>romain_lettuce</x:t>
-  </x:si>
-  <x:si>
-    <x:t>minestrone_soup</x:t>
-  </x:si>
-  <x:si>
-    <x:t>caprese_salad</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ingredient_id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>nutrition_id</x:t>
-  </x:si>
-  <x:si>
-    <x:t>caesar_dressing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>romaine_lettuce</x:t>
-  </x:si>
-  <x:si>
-    <x:t>밀, 유제품, 견과류, 생선</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gluten</x:t>
-  </x:si>
-  <x:si>
-    <x:t>garlic</x:t>
-  </x:si>
-  <x:si>
-    <x:t>vanilla</x:t>
-  </x:si>
-  <x:si>
-    <x:t>메인디쉬</x:t>
-  </x:si>
-  <x:si>
-    <x:t>포카치아</x:t>
-  </x:si>
-  <x:si>
-    <x:t>에피타이저</x:t>
-  </x:si>
-  <x:si>
-    <x:t>재료 양</x:t>
-  </x:si>
-  <x:si>
-    <x:t>userID</x:t>
-  </x:si>
-  <x:si>
-    <x:t>rice</x:t>
-  </x:si>
-  <x:si>
-    <x:t>원두: 8g</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gelatin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>crouton</x:t>
-  </x:si>
-  <x:si>
-    <x:t>butter</x:t>
-  </x:si>
-  <x:si>
-    <x:t>cheese</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://img.freepik.com/premium-photo/photo-chicken-alfredo-pasta_933496-17781.jpg</x:t>
+    <x:t>espresso</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -729,7 +732,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -812,7 +814,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -847,7 +848,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -892,7 +892,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -936,7 +935,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1021,7 +1019,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1042,7 +1039,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1073,7 +1069,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -1441,8 +1436,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A1:H20"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D24" activeCellId="0" sqref="D24:D24"/>
+    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="C25" activeCellId="0" sqref="C25:C25"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="16.399999999999999"/>
@@ -1459,28 +1454,28 @@
   <x:sheetData>
     <x:row r="1" spans="1:8" s="3" customFormat="1">
       <x:c r="A1" s="3" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="3" t="s">
-        <x:v>22</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C1" s="9" t="s">
-        <x:v>10</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D1" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="E1" s="3" t="s">
-        <x:v>96</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="F1" s="3" t="s">
-        <x:v>148</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="G1" s="3" t="s">
-        <x:v>100</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="H1" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:8">
@@ -1488,25 +1483,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>113</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C2" s="8" t="s">
-        <x:v>147</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D2" s="2" t="s">
-        <x:v>126</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F2" s="4" t="s">
-        <x:v>15</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="G2" s="4" t="s">
-        <x:v>19</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="H2" s="5" t="s">
-        <x:v>68</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -1514,25 +1509,25 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
-        <x:v>66</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C3" s="8" t="s">
-        <x:v>147</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D3" s="2" t="s">
-        <x:v>32</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="E3" s="2" t="s">
-        <x:v>11</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F3" s="4" t="s">
-        <x:v>84</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="G3" s="4" t="s">
-        <x:v>77</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H3" s="5" t="s">
-        <x:v>87</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -1540,25 +1535,25 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
-        <x:v>94</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C4" s="8" t="s">
-        <x:v>147</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D4" s="2" t="s">
-        <x:v>125</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E4" s="2" t="s">
-        <x:v>62</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F4" s="4" t="s">
-        <x:v>13</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G4" s="4" t="s">
-        <x:v>81</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="H4" s="5" t="s">
-        <x:v>88</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:8" s="4" customFormat="1">
@@ -1566,25 +1561,25 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
-        <x:v>40</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C5" s="8" t="s">
-        <x:v>145</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D5" s="2" t="s">
-        <x:v>35</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E5" s="2" t="s">
-        <x:v>99</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="F5" s="4" t="s">
-        <x:v>83</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G5" s="4" t="s">
-        <x:v>75</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H5" s="5" t="s">
-        <x:v>69</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:8" s="4" customFormat="1">
@@ -1592,25 +1587,25 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
-        <x:v>51</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C6" s="8" t="s">
-        <x:v>145</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D6" s="2" t="s">
-        <x:v>128</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E6" s="2" t="s">
-        <x:v>52</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="F6" s="4" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="G6" s="4" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="H6" s="5" t="s">
         <x:v>26</x:v>
-      </x:c>
-      <x:c r="G6" s="4" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="H6" s="5" t="s">
-        <x:v>156</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:8" s="4" customFormat="1">
@@ -1618,25 +1613,25 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="2" t="s">
-        <x:v>67</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C7" s="8" t="s">
-        <x:v>145</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D7" s="2" t="s">
-        <x:v>124</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E7" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F7" s="4" t="s">
-        <x:v>79</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G7" s="4" t="s">
-        <x:v>78</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="H7" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:8" s="4" customFormat="1">
@@ -1644,25 +1639,25 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="2" t="s">
-        <x:v>95</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C8" s="8" t="s">
-        <x:v>145</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D8" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E8" s="2" t="s">
-        <x:v>141</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F8" s="4" t="s">
-        <x:v>17</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="G8" s="4" t="s">
-        <x:v>80</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H8" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:8" s="4" customFormat="1">
@@ -1670,25 +1665,25 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="2" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="C9" s="8" t="s">
-        <x:v>145</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D9" s="2" t="s">
-        <x:v>31</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E9" s="2" t="s">
-        <x:v>63</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F9" s="4" t="s">
-        <x:v>71</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G9" s="4" t="s">
-        <x:v>76</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="H9" s="5" t="s">
-        <x:v>89</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:8" s="4" customFormat="1">
@@ -1696,25 +1691,25 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="2" t="s">
-        <x:v>146</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="C10" s="8" t="s">
-        <x:v>145</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D10" s="2" t="s">
-        <x:v>37</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="E10" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="F10" s="4" t="s">
-        <x:v>123</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G10" s="4" t="s">
-        <x:v>18</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="H10" s="5" t="s">
-        <x:v>82</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:8" s="4" customFormat="1">
@@ -1722,25 +1717,25 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="2" t="s">
-        <x:v>48</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C11" s="8" t="s">
-        <x:v>145</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D11" s="2" t="s">
-        <x:v>30</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E11" s="2" t="s">
-        <x:v>111</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F11" s="4" t="s">
-        <x:v>72</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="G11" s="4" t="s">
-        <x:v>16</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="H11" s="5" t="s">
-        <x:v>85</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:8" s="4" customFormat="1">
@@ -1748,25 +1743,25 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="2" t="s">
-        <x:v>5</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="C12" s="8" t="s">
-        <x:v>8</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="D12" s="2" t="s">
-        <x:v>133</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E12" s="2" t="s">
-        <x:v>49</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="F12" s="4" t="s">
-        <x:v>27</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G12" s="4" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H12" s="5" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="H12" s="5" t="s">
-        <x:v>70</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:8" s="4" customFormat="1">
@@ -1774,25 +1769,25 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="2" t="s">
-        <x:v>101</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C13" s="8" t="s">
-        <x:v>8</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="D13" s="2" t="s">
-        <x:v>34</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E13" s="2" t="s">
-        <x:v>11</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="F13" s="4" t="s">
-        <x:v>28</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="G13" s="4" t="s">
-        <x:v>12</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="H13" s="5" t="s">
-        <x:v>90</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:8" s="4" customFormat="1">
@@ -1800,30 +1795,30 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="2" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="C14" s="8" t="s">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="E14" s="2" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="F14" s="4" t="s">
         <x:v>98</x:v>
       </x:c>
-      <x:c r="C14" s="8" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D14" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="E14" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F14" s="4" t="s">
-        <x:v>151</x:v>
-      </x:c>
       <x:c r="G14" s="4" t="s">
-        <x:v>73</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="H14" s="5" t="s">
-        <x:v>86</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="2:2">
       <x:c r="B20" s="12" t="s">
-        <x:v>21</x:v>
+        <x:v>36</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1863,37 +1858,37 @@
   <x:sheetData>
     <x:row r="1" spans="1:12" s="7" customFormat="1">
       <x:c r="A1" s="7" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="9" t="s">
-        <x:v>149</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C1" s="9" t="s">
-        <x:v>142</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D1" s="9" t="s">
-        <x:v>93</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="E1" s="9" t="s">
-        <x:v>7</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="F1" s="9" t="s">
-        <x:v>64</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="G1" s="9" t="s">
-        <x:v>4</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="H1" s="9" t="s">
-        <x:v>9</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="I1" s="9" t="s">
-        <x:v>108</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="J1" s="9" t="s">
-        <x:v>121</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="K1" s="9" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="L1" s="9" t="s">
         <x:v>122</x:v>
@@ -1904,7 +1899,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="8" t="s">
-        <x:v>102</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C2" s="8" t="b">
         <x:v>0</x:v>
@@ -1962,7 +1957,7 @@
   <x:dimension ref="A1:AB2"/>
   <x:sheetViews>
     <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="AB1" activeCellId="0" sqref="A1:AB2"/>
+      <x:selection activeCell="F2" activeCellId="0" sqref="F2:F2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="16.399999999999999"/>
@@ -1976,88 +1971,88 @@
   <x:sheetData>
     <x:row r="1" spans="1:28" s="9" customFormat="1">
       <x:c r="A1" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="9" t="s">
-        <x:v>53</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C1" s="9" t="s">
-        <x:v>105</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D1" s="9" t="s">
-        <x:v>112</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="E1" s="9" t="s">
-        <x:v>50</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F1" s="9" t="s">
-        <x:v>143</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G1" s="9" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="H1" s="9" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="I1" s="9" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="J1" s="9" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="K1" s="9" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="L1" s="9" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="M1" s="9" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="N1" s="9" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="O1" s="9" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="P1" s="9" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="Q1" s="9" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="R1" s="9" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="S1" s="9" t="s">
         <x:v>155</x:v>
       </x:c>
-      <x:c r="H1" s="9" t="s">
-        <x:v>116</x:v>
-      </x:c>
-      <x:c r="I1" s="9" t="s">
-        <x:v>131</x:v>
-      </x:c>
-      <x:c r="J1" s="9" t="s">
-        <x:v>104</x:v>
-      </x:c>
-      <x:c r="K1" s="9" t="s">
-        <x:v>154</x:v>
-      </x:c>
-      <x:c r="L1" s="9" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="M1" s="9" t="s">
-        <x:v>115</x:v>
-      </x:c>
-      <x:c r="N1" s="9" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="O1" s="9" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="P1" s="9" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="Q1" s="9" t="s">
-        <x:v>117</x:v>
-      </x:c>
-      <x:c r="R1" s="9" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="S1" s="9" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="T1" s="9" t="s">
-        <x:v>144</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="U1" s="9" t="s">
-        <x:v>152</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="V1" s="9" t="s">
-        <x:v>39</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="W1" s="9" t="s">
-        <x:v>140</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="X1" s="9" t="s">
-        <x:v>153</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="Y1" s="9" t="s">
-        <x:v>139</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="Z1" s="9" t="s">
-        <x:v>92</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="AA1" s="9" t="s">
-        <x:v>121</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="AB1" s="9" t="s">
-        <x:v>42</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:28" s="6" customFormat="1">
@@ -2157,8 +2152,8 @@
   <x:sheetPr codeName="Sheet2"/>
   <x:dimension ref="A1:O21"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="O1" activeCellId="0" sqref="A1:O2"/>
+    <x:sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="N7" activeCellId="0" sqref="N7:N7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="16.399999999999999"/>
@@ -2181,49 +2176,49 @@
   <x:sheetData>
     <x:row r="1" spans="1:15" s="7" customFormat="1">
       <x:c r="A1" s="7" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="3" t="s">
-        <x:v>61</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C1" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D1" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E1" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="F1" s="3" t="s">
-        <x:v>129</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="G1" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H1" s="3" t="s">
-        <x:v>45</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="I1" s="3" t="s">
-        <x:v>127</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="J1" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="K1" s="3" t="s">
-        <x:v>135</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="L1" s="3" t="s">
         <x:v>103</x:v>
       </x:c>
       <x:c r="M1" s="3" t="s">
-        <x:v>47</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="N1" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="O1" s="7" t="s">
-        <x:v>58</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:15" s="6" customFormat="1">
@@ -2342,37 +2337,37 @@
   <x:sheetData>
     <x:row r="1" spans="1:11" s="7" customFormat="1">
       <x:c r="A1" s="7" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="7" t="s">
-        <x:v>91</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C1" s="7" t="s">
-        <x:v>41</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="D1" s="9" t="s">
-        <x:v>137</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E1" s="9" t="s">
-        <x:v>54</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F1" s="9" t="s">
-        <x:v>138</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G1" s="9" t="s">
-        <x:v>59</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="H1" s="9" t="s">
-        <x:v>33</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="I1" s="7" t="s">
-        <x:v>106</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="J1" s="9" t="s">
-        <x:v>44</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K1" s="3" t="s">
-        <x:v>43</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:11" s="6" customFormat="1">
@@ -2380,10 +2375,10 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>61</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C2" s="6" t="s">
-        <x:v>57</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="D2" s="2">
         <x:v>1</x:v>
@@ -2407,7 +2402,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K2" s="11" t="s">
-        <x:v>68</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:11" s="6" customFormat="1">
@@ -2415,10 +2410,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
-        <x:v>136</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C3" s="6" t="s">
-        <x:v>57</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="D3" s="2">
         <x:v>2</x:v>
@@ -2442,7 +2437,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K3" s="11" t="s">
-        <x:v>87</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:11" s="6" customFormat="1">
@@ -2450,10 +2445,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
-        <x:v>132</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C4" s="6" t="s">
-        <x:v>57</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="D4" s="2">
         <x:v>3</x:v>
@@ -2477,7 +2472,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K4" s="11" t="s">
-        <x:v>88</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11" s="8" customFormat="1">
@@ -2485,10 +2480,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
-        <x:v>36</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="C5" s="8" t="s">
-        <x:v>46</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D5" s="2">
         <x:v>4</x:v>
@@ -2512,7 +2507,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K5" s="11" t="s">
-        <x:v>69</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:11" s="8" customFormat="1">
@@ -2520,10 +2515,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
-        <x:v>129</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C6" s="8" t="s">
-        <x:v>46</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D6" s="2">
         <x:v>5</x:v>
@@ -2547,7 +2542,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K6" s="11" t="s">
-        <x:v>156</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:11" s="8" customFormat="1">
@@ -2555,10 +2550,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="2" t="s">
-        <x:v>38</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C7" s="8" t="s">
-        <x:v>46</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D7" s="2">
         <x:v>6</x:v>
@@ -2582,7 +2577,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K7" s="11" t="s">
-        <x:v>20</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:11" s="8" customFormat="1">
@@ -2590,10 +2585,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="2" t="s">
-        <x:v>45</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C8" s="8" t="s">
-        <x:v>46</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D8" s="2">
         <x:v>7</x:v>
@@ -2617,7 +2612,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K8" s="11" t="s">
-        <x:v>25</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:11" s="8" customFormat="1">
@@ -2625,10 +2620,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="2" t="s">
-        <x:v>127</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C9" s="8" t="s">
-        <x:v>46</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D9" s="2">
         <x:v>8</x:v>
@@ -2652,7 +2647,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K9" s="11" t="s">
-        <x:v>89</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:11" s="8" customFormat="1">
@@ -2660,10 +2655,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="2" t="s">
-        <x:v>65</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C10" s="8" t="s">
-        <x:v>46</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D10" s="2">
         <x:v>9</x:v>
@@ -2687,7 +2682,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K10" s="11" t="s">
-        <x:v>82</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:11" s="8" customFormat="1">
@@ -2695,10 +2690,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="2" t="s">
-        <x:v>135</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C11" s="8" t="s">
-        <x:v>46</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="D11" s="2">
         <x:v>10</x:v>
@@ -2722,7 +2717,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K11" s="11" t="s">
-        <x:v>85</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:11" s="8" customFormat="1">
@@ -2733,7 +2728,7 @@
         <x:v>103</x:v>
       </x:c>
       <x:c r="C12" s="8" t="s">
-        <x:v>107</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D12" s="2">
         <x:v>11</x:v>
@@ -2757,7 +2752,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K12" s="11" t="s">
-        <x:v>70</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:11" s="8" customFormat="1">
@@ -2765,10 +2760,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="2" t="s">
-        <x:v>47</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C13" s="8" t="s">
-        <x:v>107</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D13" s="2">
         <x:v>12</x:v>
@@ -2792,7 +2787,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K13" s="11" t="s">
-        <x:v>90</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:11" s="8" customFormat="1">
@@ -2800,10 +2795,10 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="2" t="s">
-        <x:v>56</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C14" s="8" t="s">
-        <x:v>107</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="D14" s="2">
         <x:v>13</x:v>
@@ -2827,7 +2822,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="K14" s="11" t="s">
-        <x:v>86</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2872,88 +2867,88 @@
   <x:sheetData>
     <x:row r="1" spans="1:28" s="7" customFormat="1">
       <x:c r="A1" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="9" t="s">
-        <x:v>53</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C1" s="9" t="s">
-        <x:v>105</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D1" s="7" t="s">
-        <x:v>112</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="E1" s="7" t="s">
-        <x:v>50</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F1" s="7" t="s">
-        <x:v>143</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G1" s="7" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="H1" s="7" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="I1" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="J1" s="7" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="K1" s="7" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="L1" s="7" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="M1" s="7" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="N1" s="7" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="O1" s="7" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="P1" s="7" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="Q1" s="7" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="R1" s="7" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="S1" s="7" t="s">
         <x:v>155</x:v>
       </x:c>
-      <x:c r="H1" s="7" t="s">
-        <x:v>116</x:v>
-      </x:c>
-      <x:c r="I1" s="7" t="s">
-        <x:v>131</x:v>
-      </x:c>
-      <x:c r="J1" s="7" t="s">
-        <x:v>104</x:v>
-      </x:c>
-      <x:c r="K1" s="7" t="s">
-        <x:v>154</x:v>
-      </x:c>
-      <x:c r="L1" s="7" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="M1" s="7" t="s">
-        <x:v>115</x:v>
-      </x:c>
-      <x:c r="N1" s="7" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="O1" s="7" t="s">
-        <x:v>150</x:v>
-      </x:c>
-      <x:c r="P1" s="7" t="s">
-        <x:v>118</x:v>
-      </x:c>
-      <x:c r="Q1" s="7" t="s">
-        <x:v>117</x:v>
-      </x:c>
-      <x:c r="R1" s="7" t="s">
-        <x:v>119</x:v>
-      </x:c>
-      <x:c r="S1" s="7" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="T1" s="7" t="s">
-        <x:v>144</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="U1" s="7" t="s">
-        <x:v>152</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="V1" s="7" t="s">
-        <x:v>39</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="W1" s="7" t="s">
-        <x:v>134</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="X1" s="7" t="s">
-        <x:v>153</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="Y1" s="7" t="s">
-        <x:v>139</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="Z1" s="7" t="s">
-        <x:v>92</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="AA1" s="7" t="s">
-        <x:v>121</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="AB1" s="7" t="s">
-        <x:v>42</x:v>
+        <x:v>74</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:29" s="6" customFormat="1">
@@ -4104,34 +4099,34 @@
   <x:sheetData>
     <x:row r="1" spans="1:10" s="7" customFormat="1">
       <x:c r="A1" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="7" t="s">
-        <x:v>142</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C1" s="7" t="s">
-        <x:v>93</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="D1" s="7" t="s">
-        <x:v>7</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="E1" s="7" t="s">
-        <x:v>64</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F1" s="7" t="s">
-        <x:v>4</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G1" s="7" t="s">
-        <x:v>9</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="H1" s="7" t="s">
-        <x:v>108</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="I1" s="7" t="s">
-        <x:v>121</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="J1" s="7" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:10" s="6" customFormat="1">
@@ -4574,22 +4569,22 @@
   <x:sheetData>
     <x:row r="1" spans="1:6" s="7" customFormat="1">
       <x:c r="A1" s="9" t="s">
-        <x:v>6</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B1" s="7" t="s">
-        <x:v>130</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C1" s="7" t="s">
-        <x:v>110</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="D1" s="7" t="s">
-        <x:v>3</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="E1" s="7" t="s">
-        <x:v>114</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F1" s="7" t="s">
-        <x:v>55</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6" s="6" customFormat="1">

</xml_diff>